<commit_message>
Added cow birth status
</commit_message>
<xml_diff>
--- a/DairyRecordKeeping.xlsx
+++ b/DairyRecordKeeping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pjd\Dairy_git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF084472-E48C-42D5-9998-A10540F5D12A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03242FF1-2705-4280-BC8B-2A87F5A6F6AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="603" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,6 +37,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2747" uniqueCount="593">
   <si>
     <t>UP</t>
   </si>
@@ -1822,6 +1823,20 @@
   <si>
     <t>2/10/2018
 24-oct-2019</t>
+  </si>
+  <si>
+    <t>From boopathy</t>
+  </si>
+  <si>
+    <t>15/6/2018
+4/11/2019</t>
+  </si>
+  <si>
+    <t>Female
+Male</t>
+  </si>
+  <si>
+    <t>Sold</t>
   </si>
 </sst>
 </file>
@@ -2195,6 +2210,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2209,9 +2227,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4650,24 +4665,24 @@
       <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="68" t="s">
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="69" t="s">
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
@@ -4822,18 +4837,18 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C18" s="70" t="s">
+      <c r="C18" s="71" t="s">
         <v>251</v>
       </c>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="I18" s="70" t="s">
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="I18" s="71" t="s">
         <v>252</v>
       </c>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="71"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E19" s="24" t="s">
@@ -7066,7 +7081,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7265,8 +7280,8 @@
       <c r="A7" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>111</v>
+      <c r="B7" s="60" t="s">
+        <v>590</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>499</v>
@@ -7274,8 +7289,8 @@
       <c r="F7" s="59" t="s">
         <v>560</v>
       </c>
-      <c r="G7" t="s">
-        <v>307</v>
+      <c r="G7" s="13" t="s">
+        <v>591</v>
       </c>
       <c r="H7">
         <v>58000</v>
@@ -7287,12 +7302,15 @@
         <v>583</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="38.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>228</v>
       </c>
       <c r="B8" s="20">
         <v>43319</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>592</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>547</v>
@@ -7346,7 +7364,7 @@
       <c r="A10" t="s">
         <v>362</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="67" t="s">
         <v>588</v>
       </c>
       <c r="E10" s="61">
@@ -7355,8 +7373,8 @@
       <c r="F10" s="61">
         <v>43776</v>
       </c>
-      <c r="G10" t="s">
-        <v>307</v>
+      <c r="G10" s="13" t="s">
+        <v>591</v>
       </c>
       <c r="H10">
         <v>52500</v>
@@ -20631,15 +20649,15 @@
       <c r="J81" s="13"/>
       <c r="K81" s="13"/>
       <c r="L81" s="13"/>
-      <c r="M81" s="71">
+      <c r="M81" s="72">
         <f>SUM(M83:R83)</f>
         <v>56.75</v>
       </c>
-      <c r="N81" s="71"/>
-      <c r="O81" s="71"/>
-      <c r="P81" s="71"/>
-      <c r="Q81" s="71"/>
-      <c r="R81" s="71"/>
+      <c r="N81" s="72"/>
+      <c r="O81" s="72"/>
+      <c r="P81" s="72"/>
+      <c r="Q81" s="72"/>
+      <c r="R81" s="72"/>
     </row>
     <row r="82" spans="1:24" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="s">
@@ -20720,7 +20738,7 @@
       <c r="A84" s="20">
         <v>43198</v>
       </c>
-      <c r="I84" s="71"/>
+      <c r="I84" s="72"/>
       <c r="J84" s="51"/>
       <c r="K84" s="57"/>
       <c r="L84" s="64"/>
@@ -20741,7 +20759,7 @@
       <c r="H85">
         <v>4.5</v>
       </c>
-      <c r="I85" s="71"/>
+      <c r="I85" s="72"/>
       <c r="J85" s="51"/>
       <c r="K85" s="57"/>
       <c r="L85" s="64"/>
@@ -48829,57 +48847,112 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A4:J75"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="98" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="98" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1">
+        <f>SUM(C2:C100)</f>
+        <v>252082</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>455</v>
+      </c>
+      <c r="G1">
+        <f>SUM(G2:G50)</f>
+        <v>207000</v>
+      </c>
+      <c r="I1" t="s">
+        <v>456</v>
+      </c>
+      <c r="J1">
+        <f>G1-C1</f>
+        <v>-45082</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C2">
+        <v>410</v>
+      </c>
+      <c r="F2" t="s">
+        <v>450</v>
+      </c>
+      <c r="G2">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C3">
+        <v>12000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F3" t="s">
+        <v>451</v>
+      </c>
+      <c r="G3">
+        <v>12000</v>
+      </c>
+    </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="24" t="s">
-        <v>249</v>
+      <c r="A4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B4" t="s">
+        <v>442</v>
       </c>
       <c r="C4">
-        <f>SUM(C5:C91)</f>
-        <v>238882</v>
-      </c>
-      <c r="F4" s="55" t="s">
-        <v>455</v>
+        <v>500</v>
+      </c>
+      <c r="F4" t="s">
+        <v>452</v>
       </c>
       <c r="G4">
-        <f>SUM(G5:G18)</f>
-        <v>192000</v>
-      </c>
-      <c r="I4" t="s">
-        <v>456</v>
-      </c>
-      <c r="J4">
-        <f>G4-C4</f>
-        <v>-46882</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B5" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C5">
-        <v>410</v>
+        <v>-100</v>
       </c>
       <c r="F5" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="G5">
         <v>12000</v>
@@ -48887,19 +48960,19 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="B6" t="s">
         <v>441</v>
       </c>
       <c r="C6">
-        <v>12000</v>
+        <v>8000</v>
       </c>
       <c r="D6" t="s">
         <v>449</v>
       </c>
       <c r="F6" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="G6">
         <v>12000</v>
@@ -48907,7 +48980,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B7" t="s">
         <v>442</v>
@@ -48916,7 +48989,7 @@
         <v>500</v>
       </c>
       <c r="F7" t="s">
-        <v>452</v>
+        <v>532</v>
       </c>
       <c r="G7">
         <v>12000</v>
@@ -48924,64 +48997,70 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B8" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C8">
-        <v>-100</v>
+        <v>500</v>
+      </c>
+      <c r="D8" t="s">
+        <v>580</v>
       </c>
       <c r="F8" t="s">
-        <v>453</v>
+        <v>561</v>
       </c>
       <c r="G8">
-        <v>12000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B9" t="s">
         <v>441</v>
       </c>
       <c r="C9">
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="D9" t="s">
         <v>449</v>
       </c>
       <c r="F9" t="s">
-        <v>454</v>
+        <v>568</v>
       </c>
       <c r="G9">
-        <v>12000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="B10" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C10">
-        <v>500</v>
+        <v>187</v>
+      </c>
+      <c r="D10" t="s">
+        <v>580</v>
       </c>
       <c r="F10" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="G10">
-        <v>12000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C11">
         <v>500</v>
@@ -48990,7 +49069,7 @@
         <v>580</v>
       </c>
       <c r="F11" t="s">
-        <v>561</v>
+        <v>585</v>
       </c>
       <c r="G11">
         <v>15000</v>
@@ -48998,19 +49077,19 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B12" t="s">
         <v>441</v>
       </c>
       <c r="C12">
-        <v>10000</v>
+        <v>300</v>
       </c>
       <c r="D12" t="s">
-        <v>449</v>
+        <v>580</v>
       </c>
       <c r="F12" t="s">
-        <v>568</v>
+        <v>586</v>
       </c>
       <c r="G12">
         <v>15000</v>
@@ -49018,19 +49097,19 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B13" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C13">
-        <v>187</v>
+        <v>500</v>
       </c>
       <c r="D13" t="s">
         <v>580</v>
       </c>
       <c r="F13" t="s">
-        <v>576</v>
+        <v>587</v>
       </c>
       <c r="G13">
         <v>15000</v>
@@ -49038,19 +49117,19 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B14" t="s">
         <v>441</v>
       </c>
       <c r="C14">
-        <v>500</v>
+        <v>7000</v>
       </c>
       <c r="D14" t="s">
-        <v>580</v>
+        <v>449</v>
       </c>
       <c r="F14" t="s">
-        <v>585</v>
+        <v>450</v>
       </c>
       <c r="G14">
         <v>15000</v>
@@ -49058,7 +49137,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B15" t="s">
         <v>441</v>
@@ -49070,7 +49149,7 @@
         <v>580</v>
       </c>
       <c r="F15" t="s">
-        <v>586</v>
+        <v>451</v>
       </c>
       <c r="G15">
         <v>15000</v>
@@ -49078,267 +49157,249 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B16" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C16">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="D16" t="s">
         <v>580</v>
       </c>
       <c r="F16" t="s">
-        <v>587</v>
+        <v>452</v>
       </c>
       <c r="G16">
         <v>15000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B17" t="s">
         <v>441</v>
       </c>
       <c r="C17">
-        <v>7000</v>
+        <v>2000</v>
       </c>
       <c r="D17" t="s">
-        <v>449</v>
+        <v>580</v>
       </c>
       <c r="F17" t="s">
-        <v>450</v>
-      </c>
-      <c r="G17">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B18" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="C18">
-        <v>300</v>
+        <v>-500</v>
       </c>
       <c r="D18" t="s">
         <v>580</v>
       </c>
       <c r="F18" t="s">
-        <v>451</v>
-      </c>
-      <c r="G18">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B19" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C19">
-        <v>800</v>
+        <v>-200</v>
       </c>
       <c r="D19" t="s">
         <v>580</v>
       </c>
-      <c r="F19" t="s">
-        <v>452</v>
-      </c>
-      <c r="G19">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B20" t="s">
         <v>441</v>
       </c>
       <c r="C20">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="D20" t="s">
         <v>580</v>
       </c>
-      <c r="F20" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="B21" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C21">
-        <v>-500</v>
+        <v>10000</v>
       </c>
       <c r="D21" t="s">
-        <v>580</v>
-      </c>
-      <c r="F21" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="B22" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C22">
-        <v>-200</v>
+        <v>2000</v>
       </c>
       <c r="D22" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B23" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="C23">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D23" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="B24" t="s">
         <v>441</v>
       </c>
       <c r="C24">
-        <v>10000</v>
+        <v>700</v>
       </c>
       <c r="D24" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B25" t="s">
         <v>441</v>
       </c>
       <c r="C25">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="D25" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B26" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="C26">
-        <v>300</v>
+        <v>10000</v>
       </c>
       <c r="D26" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B27" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="C27">
-        <v>700</v>
+        <v>1880</v>
       </c>
       <c r="D27" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B28" t="s">
         <v>441</v>
       </c>
       <c r="C28">
-        <v>500</v>
+        <v>5000</v>
       </c>
       <c r="D28" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B29" t="s">
         <v>441</v>
       </c>
       <c r="C29">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="D29" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B30" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="C30">
-        <v>1880</v>
+        <v>100</v>
       </c>
       <c r="D30" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B31" t="s">
         <v>441</v>
       </c>
       <c r="C31">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="D31" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B32" t="s">
         <v>441</v>
       </c>
       <c r="C32">
-        <v>2000</v>
+        <v>2200</v>
       </c>
       <c r="D32" t="s">
         <v>580</v>
@@ -49346,13 +49407,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B33" t="s">
         <v>441</v>
       </c>
       <c r="C33">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D33" t="s">
         <v>580</v>
@@ -49360,7 +49421,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B34" t="s">
         <v>441</v>
@@ -49374,21 +49435,21 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>437</v>
+        <v>480</v>
       </c>
       <c r="B35" t="s">
         <v>441</v>
       </c>
       <c r="C35">
-        <v>2200</v>
+        <v>7000</v>
       </c>
       <c r="D35" t="s">
-        <v>580</v>
+        <v>449</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>438</v>
+        <v>479</v>
       </c>
       <c r="B36" t="s">
         <v>441</v>
@@ -49399,16 +49460,19 @@
       <c r="D36" t="s">
         <v>580</v>
       </c>
+      <c r="E36" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>439</v>
+        <v>479</v>
       </c>
       <c r="B37" t="s">
         <v>441</v>
       </c>
       <c r="C37">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="D37" t="s">
         <v>580</v>
@@ -49416,21 +49480,21 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>480</v>
+        <v>533</v>
       </c>
       <c r="B38" t="s">
         <v>441</v>
       </c>
       <c r="C38">
-        <v>7000</v>
+        <v>1000</v>
       </c>
       <c r="D38" t="s">
-        <v>449</v>
+        <v>580</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>479</v>
+        <v>534</v>
       </c>
       <c r="B39" t="s">
         <v>441</v>
@@ -49441,19 +49505,16 @@
       <c r="D39" t="s">
         <v>580</v>
       </c>
-      <c r="E39" t="s">
-        <v>495</v>
-      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>479</v>
+        <v>535</v>
       </c>
       <c r="B40" t="s">
         <v>441</v>
       </c>
       <c r="C40">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="D40" t="s">
         <v>580</v>
@@ -49461,13 +49522,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B41" t="s">
         <v>441</v>
       </c>
       <c r="C41">
-        <v>1000</v>
+        <v>7000</v>
       </c>
       <c r="D41" t="s">
         <v>580</v>
@@ -49475,13 +49536,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B42" t="s">
         <v>441</v>
       </c>
       <c r="C42">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="D42" t="s">
         <v>580</v>
@@ -49489,7 +49550,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="B43" t="s">
         <v>441</v>
@@ -49503,13 +49564,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>536</v>
+        <v>570</v>
       </c>
       <c r="B44" t="s">
         <v>441</v>
       </c>
       <c r="C44">
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="D44" t="s">
         <v>580</v>
@@ -49517,7 +49578,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>536</v>
+        <v>570</v>
       </c>
       <c r="B45" t="s">
         <v>441</v>
@@ -49531,13 +49592,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>537</v>
+        <v>571</v>
       </c>
       <c r="B46" t="s">
         <v>441</v>
       </c>
       <c r="C46">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="D46" t="s">
         <v>580</v>
@@ -49545,49 +49606,52 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B47" t="s">
         <v>441</v>
       </c>
       <c r="C47">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="D47" t="s">
         <v>580</v>
       </c>
+      <c r="E47" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B48" t="s">
         <v>441</v>
       </c>
       <c r="C48">
-        <v>1000</v>
+        <v>4000</v>
       </c>
       <c r="D48" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B49" t="s">
         <v>441</v>
       </c>
       <c r="C49">
-        <v>1000</v>
+        <v>7000</v>
       </c>
       <c r="D49" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="B50" t="s">
         <v>441</v>
@@ -49598,238 +49662,325 @@
       <c r="D50" t="s">
         <v>580</v>
       </c>
-      <c r="E50" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>569</v>
+        <v>577</v>
       </c>
       <c r="B51" t="s">
         <v>441</v>
       </c>
       <c r="C51">
-        <v>4000</v>
+        <v>7000</v>
       </c>
       <c r="D51" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>569</v>
+        <v>578</v>
       </c>
       <c r="B52" t="s">
         <v>441</v>
       </c>
       <c r="C52">
-        <v>7000</v>
+        <v>5000</v>
       </c>
       <c r="D52" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="B53" t="s">
         <v>441</v>
       </c>
       <c r="C53">
-        <v>500</v>
+        <v>2255</v>
       </c>
       <c r="D53" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>577</v>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="61">
+        <v>43611</v>
+      </c>
+      <c r="B54" t="s">
+        <v>441</v>
       </c>
       <c r="C54">
-        <v>7000</v>
+        <v>300</v>
       </c>
       <c r="D54" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>578</v>
+        <v>580</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="61">
+        <v>43611</v>
+      </c>
+      <c r="B55" t="s">
+        <v>441</v>
       </c>
       <c r="C55">
-        <v>5000</v>
+        <v>700</v>
       </c>
       <c r="D55" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>579</v>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="61">
+        <v>43617</v>
+      </c>
+      <c r="B56" t="s">
+        <v>441</v>
       </c>
       <c r="C56">
-        <v>2255</v>
+        <v>150</v>
       </c>
       <c r="D56" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="61">
-        <v>43611</v>
+        <v>43617</v>
+      </c>
+      <c r="B57" t="s">
+        <v>441</v>
       </c>
       <c r="C57">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="D57" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="61">
-        <v>43611</v>
+        <v>43617</v>
+      </c>
+      <c r="B58" t="s">
+        <v>441</v>
       </c>
       <c r="C58">
+        <v>12000</v>
+      </c>
+      <c r="D58" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="61">
+        <v>43624</v>
+      </c>
+      <c r="B59" t="s">
+        <v>441</v>
+      </c>
+      <c r="C59">
+        <v>500</v>
+      </c>
+      <c r="D59" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="61">
+        <v>43631</v>
+      </c>
+      <c r="B60" t="s">
+        <v>441</v>
+      </c>
+      <c r="C60">
+        <v>1000</v>
+      </c>
+      <c r="D60" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="61">
+        <v>43646</v>
+      </c>
+      <c r="B61" t="s">
+        <v>441</v>
+      </c>
+      <c r="C61">
+        <v>3000</v>
+      </c>
+      <c r="D61" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="61">
+        <v>43646</v>
+      </c>
+      <c r="B62" t="s">
+        <v>441</v>
+      </c>
+      <c r="C62">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="61">
+        <v>43656</v>
+      </c>
+      <c r="B63" t="s">
+        <v>441</v>
+      </c>
+      <c r="C63">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="61">
+        <v>43678</v>
+      </c>
+      <c r="B64" t="s">
+        <v>441</v>
+      </c>
+      <c r="C64">
+        <v>8000</v>
+      </c>
+      <c r="D64" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="61">
+        <v>43681</v>
+      </c>
+      <c r="B65" t="s">
+        <v>441</v>
+      </c>
+      <c r="C65">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="61">
+        <v>43694</v>
+      </c>
+      <c r="B66" t="s">
+        <v>441</v>
+      </c>
+      <c r="C66">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="61">
+        <v>43701</v>
+      </c>
+      <c r="B67" t="s">
+        <v>441</v>
+      </c>
+      <c r="C67">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="61">
+        <v>43711</v>
+      </c>
+      <c r="B68" t="s">
+        <v>441</v>
+      </c>
+      <c r="C68">
+        <v>12000</v>
+      </c>
+      <c r="D68" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="61">
+        <v>43722</v>
+      </c>
+      <c r="B69" t="s">
+        <v>441</v>
+      </c>
+      <c r="C69">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="61">
+        <v>43729</v>
+      </c>
+      <c r="B70" t="s">
+        <v>441</v>
+      </c>
+      <c r="C70">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="61">
+        <v>43737</v>
+      </c>
+      <c r="B71" t="s">
+        <v>441</v>
+      </c>
+      <c r="C71">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="61">
+        <v>43739</v>
+      </c>
+      <c r="B72" t="s">
+        <v>441</v>
+      </c>
+      <c r="C72">
+        <v>7000</v>
+      </c>
+      <c r="D72" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="61">
+        <v>43758</v>
+      </c>
+      <c r="B73" t="s">
+        <v>441</v>
+      </c>
+      <c r="C73">
         <v>700</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="61">
-        <v>43617</v>
-      </c>
-      <c r="C59">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="61">
-        <v>43617</v>
-      </c>
-      <c r="C60">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="61">
-        <v>43617</v>
-      </c>
-      <c r="C61">
+      <c r="D73" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="61">
+        <v>43770</v>
+      </c>
+      <c r="C74">
         <v>12000</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="61">
-        <v>43624</v>
-      </c>
-      <c r="C62">
+      <c r="D74" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="61">
+        <v>43770</v>
+      </c>
+      <c r="C75">
         <v>500</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" s="61">
-        <v>43631</v>
-      </c>
-      <c r="C63">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="61">
-        <v>43646</v>
-      </c>
-      <c r="C64">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="61">
-        <v>43646</v>
-      </c>
-      <c r="C65">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="61">
-        <v>43656</v>
-      </c>
-      <c r="C66">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="61">
-        <v>43678</v>
-      </c>
-      <c r="C67">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="61">
-        <v>43681</v>
-      </c>
-      <c r="C68">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="61">
-        <v>43694</v>
-      </c>
-      <c r="C69">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="61">
-        <v>43701</v>
-      </c>
-      <c r="C70">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="61">
-        <v>43711</v>
-      </c>
-      <c r="C71">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="61">
-        <v>43722</v>
-      </c>
-      <c r="C72">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="61">
-        <v>43729</v>
-      </c>
-      <c r="C73">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="61">
-        <v>43737</v>
-      </c>
-      <c r="C74">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="61">
-        <v>43739</v>
-      </c>
-      <c r="C75">
-        <v>7000</v>
+      <c r="D75" t="s">
+        <v>580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>